<commit_message>
Added results to spreadsheet
</commit_message>
<xml_diff>
--- a/Results_Spreadsheet.xlsx
+++ b/Results_Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\BCB546\Group Project\BCB546X_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3276FCB-EED9-4401-B42F-AD8A1CFF2B84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5CFFDE4-7260-4F8D-BDD8-6BA5EF39AF41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FDF7948-A049-4EF5-95C9-622BE3889573}"/>
   </bookViews>
@@ -114,13 +114,13 @@
     <t>Our Total #s</t>
   </si>
   <si>
-    <t>Counting Uniqs</t>
-  </si>
-  <si>
     <t>Mega</t>
   </si>
   <si>
     <t>Discont.</t>
+  </si>
+  <si>
+    <t>Counting Uniqs Only - "Them" Row is our total</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CDA04D-563A-4A33-B4D6-3863C5F3B6C8}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,7 +596,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -633,9 +633,6 @@
       <c r="E8">
         <v>2</v>
       </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -651,6 +648,9 @@
         <v>15</v>
       </c>
       <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
         <v>5</v>
       </c>
     </row>
@@ -929,7 +929,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
@@ -954,7 +954,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -962,13 +962,16 @@
       <c r="D27" t="s">
         <v>15</v>
       </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -979,7 +982,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -993,7 +996,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1001,13 +1004,16 @@
       <c r="D30" t="s">
         <v>18</v>
       </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>
@@ -1018,7 +1024,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -1027,12 +1033,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -1040,13 +1046,16 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
         <v>22</v>
@@ -1055,9 +1064,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
@@ -1066,12 +1075,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
@@ -1079,13 +1088,16 @@
       <c r="D36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -1093,10 +1105,16 @@
       <c r="D37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>10004</v>
+      </c>
+      <c r="G37">
+        <v>9975</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -1104,13 +1122,19 @@
       <c r="D38" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>9960</v>
+      </c>
+      <c r="G38">
+        <v>9916</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
@@ -1118,13 +1142,24 @@
       <c r="D39" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>19891</v>
+      </c>
+      <c r="F39">
+        <f>SUM(E37:E38)</f>
+        <v>19964</v>
+      </c>
+      <c r="G39">
+        <f>SUM(G37:G38)</f>
+        <v>19891</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
         <v>24</v>
@@ -1132,10 +1167,16 @@
       <c r="D40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>380</v>
+      </c>
+      <c r="G40">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
@@ -1143,13 +1184,19 @@
       <c r="D41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>375</v>
+      </c>
+      <c r="G41">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
         <v>16</v>
@@ -1157,13 +1204,24 @@
       <c r="D42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>755</v>
+      </c>
+      <c r="F42">
+        <f>SUM(E40:E41)</f>
+        <v>755</v>
+      </c>
+      <c r="G42">
+        <f>SUM(G40:G41)</f>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -1172,9 +1230,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>20</v>
@@ -1183,12 +1241,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
@@ -1196,13 +1254,16 @@
       <c r="D45" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -1211,9 +1272,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
@@ -1222,12 +1283,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -1235,13 +1296,16 @@
       <c r="D48" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
         <v>22</v>
@@ -1250,9 +1314,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
         <v>23</v>
@@ -1261,12 +1325,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
@@ -1274,13 +1338,16 @@
       <c r="D51" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" t="s">
         <v>22</v>
@@ -1289,9 +1356,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
@@ -1300,12 +1367,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
@@ -1313,13 +1380,16 @@
       <c r="D54" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
         <v>24</v>
@@ -1327,10 +1397,16 @@
       <c r="D55" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>10004</v>
+      </c>
+      <c r="G55">
+        <v>9975</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
@@ -1338,13 +1414,19 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>9960</v>
+      </c>
+      <c r="G56">
+        <v>9916</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
@@ -1352,13 +1434,24 @@
       <c r="D57" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>19917</v>
+      </c>
+      <c r="F57">
+        <f>SUM(E55:E56)</f>
+        <v>19964</v>
+      </c>
+      <c r="G57">
+        <f>SUM(G55:G56)</f>
+        <v>19891</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C58" t="s">
         <v>24</v>
@@ -1366,10 +1459,16 @@
       <c r="D58" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>380</v>
+      </c>
+      <c r="G58">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -1377,19 +1476,36 @@
       <c r="D59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>379</v>
+      </c>
+      <c r="G59">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
         <v>16</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
+      </c>
+      <c r="E60">
+        <v>759</v>
+      </c>
+      <c r="F60">
+        <f>SUM(E58:E59)</f>
+        <v>759</v>
+      </c>
+      <c r="G60">
+        <f>SUM(G58:G59)</f>
+        <v>759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>